<commit_message>
Update 04 Diseno de Mapa de Competencias.xlsx
</commit_message>
<xml_diff>
--- a/04 Diseno de Mapa de Competencias.xlsx
+++ b/04 Diseno de Mapa de Competencias.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaven\Documents\GitHub\cdia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196007F3-3E28-4775-883F-D97D85B8B512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BCDDDA-E99C-4D39-B32E-9DEE5BDB798D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MACROCOMPETENCIA 1" sheetId="2" r:id="rId1"/>
     <sheet name="MACROCOMPETENCIA 2" sheetId="5" r:id="rId2"/>
     <sheet name="MACROCOMPETENCIA 3" sheetId="6" r:id="rId3"/>
-    <sheet name="MACROCOMPETENCIA - PLANTILLA" sheetId="1" r:id="rId4"/>
+    <sheet name="ABET - rel" sheetId="7" r:id="rId4"/>
+    <sheet name="MACROCOMPETENCIA - PLANTILLA" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -230,7 +231,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="149">
   <si>
     <t>MACRO-COMPETENCIA (MC)</t>
   </si>
@@ -404,24 +405,15 @@
     <t>Explica</t>
   </si>
   <si>
-    <t>los principios y metodologías de diseño de arquitecturas de datos para analítica avanzada</t>
-  </si>
-  <si>
     <t xml:space="preserve">Construye </t>
   </si>
   <si>
-    <t>prototipos de soluciones tecnológicas que integran datos y algoritmos inteligentes para un caso de estudio</t>
-  </si>
-  <si>
     <t>la selección de algoritmos inteligentes y técnicas de analítica avanzada</t>
   </si>
   <si>
     <t>mediante la aplicación de los fundamentos de las ciencias de la computación, la estadística inferencial, la matemática aplicada, la ingeniería de software y el ciclo de vida de los datos para el cumplimiento de los requerimientos de los involucrados</t>
   </si>
   <si>
-    <t>Afinar</t>
-  </si>
-  <si>
     <t>mediante la aplicación de los fundamentos teóricos matemáticos y computacionales para el cumplimiento de los requerimientos de los involucrados</t>
   </si>
   <si>
@@ -431,9 +423,6 @@
     <t xml:space="preserve">Identifica </t>
   </si>
   <si>
-    <t>los factores que influyen en el rendimiento de los algoritmos de analítica avanzada</t>
-  </si>
-  <si>
     <t xml:space="preserve">Argumenta </t>
   </si>
   <si>
@@ -443,9 +432,6 @@
     <t xml:space="preserve">Calibra </t>
   </si>
   <si>
-    <t xml:space="preserve">parámetros de modelos de datos </t>
-  </si>
-  <si>
     <t>Implementar</t>
   </si>
   <si>
@@ -527,36 +513,12 @@
     <t xml:space="preserve">Ensambla </t>
   </si>
   <si>
-    <t>los principios de arquitectura y diseño de software para sistemas inteligentes robustos y escalables</t>
-  </si>
-  <si>
-    <t>la importancia de la colaboración en entornos multidisciplinarios para el desarrollo de sistemas tecnológicos</t>
-  </si>
-  <si>
-    <t>componentes de software para la integración de algoritmos inteligentes</t>
-  </si>
-  <si>
     <t>Aplicar</t>
   </si>
   <si>
-    <t>sistemas tecnológicos basados en datos y algoritmos inteligentes en entornos productivos</t>
-  </si>
-  <si>
-    <t>para asegurar su funcionamiento eficiente y adaptación a nuevas condiciones y problemas</t>
-  </si>
-  <si>
     <t xml:space="preserve">Monitorea </t>
   </si>
   <si>
-    <t>los requisitos técnicos y operativos para el despliegue de sistemas inteligentes</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> la necesidad de considerar aspectos éticos y legales en la adaptación de sistemas tecnológicos</t>
-  </si>
-  <si>
-    <t>el rendimiento de los sistemas implementados para garantizar su robustez y escalabilidad</t>
-  </si>
-  <si>
     <t>Evaluar</t>
   </si>
   <si>
@@ -599,27 +561,142 @@
     <t>para dar soporte en la toma de decisiones estratégicas</t>
   </si>
   <si>
-    <t>los frameworks y metodologías para la elaboración de informes de evaluación de proyectos tecnológicos</t>
-  </si>
-  <si>
     <t>la relevancia de los hallazgos de la evaluación para impulsar la innovación y la transformación digital en sectores emergentes</t>
   </si>
   <si>
     <t xml:space="preserve">Diseña </t>
   </si>
   <si>
-    <t>reportes ejecutivos que integren el análisis de datos y las simulaciones para la toma de decisiones estratégicas</t>
+    <t>Criterion 3. Student Outcomes</t>
+  </si>
+  <si>
+    <t>1. analyze a broadly defined problem in the program’s domain and apply principles of the discipline to identify solutions,</t>
+  </si>
+  <si>
+    <t>2. design and implement solutions to meet a given set of computing requirements in the context of the program’s discipline,</t>
+  </si>
+  <si>
+    <t>3. communicate effectively in a variety of professional contexts,</t>
+  </si>
+  <si>
+    <t>4. recognize professional responsibilities and make informed judgments in computing practice based on legal and ethical principles, and</t>
+  </si>
+  <si>
+    <t>5. function effectively as a member of a team engaged in activities appropriate to the program’s discipline.</t>
+  </si>
+  <si>
+    <t>1. Analizar un problema ampliamente definido en el dominio del programa y aplicar los principios de la disciplina para identificar soluciones.</t>
+  </si>
+  <si>
+    <t>2. Diseñar e implementar soluciones para satisfacer un conjunto determinado de requisitos informáticos en el contexto de la disciplina del programa.</t>
+  </si>
+  <si>
+    <t>3. Comunicarse eficazmente en diversos contextos profesionales.</t>
+  </si>
+  <si>
+    <t>4. Reconocer las responsabilidades profesionales y emitir juicios informados en la práctica informática con base en principios legales y éticos.</t>
+  </si>
+  <si>
+    <t>5. Desempeñarse eficazmente como miembro de un equipo que participa en actividades propias de la disciplina del programa.</t>
+  </si>
+  <si>
+    <t>Transversal?</t>
+  </si>
+  <si>
+    <t>Analizar un problema</t>
+  </si>
+  <si>
+    <t>Aplicar principios</t>
+  </si>
+  <si>
+    <t>Diseñar soluciones</t>
+  </si>
+  <si>
+    <t>Implementar soluciones</t>
+  </si>
+  <si>
+    <t>Reconocer responsabilidades</t>
+  </si>
+  <si>
+    <t>Emitir juicios</t>
+  </si>
+  <si>
+    <t>UC6</t>
+  </si>
+  <si>
+    <t>UC5</t>
+  </si>
+  <si>
+    <t>Análisis</t>
+  </si>
+  <si>
+    <t>Español</t>
+  </si>
+  <si>
+    <t>Inglés</t>
+  </si>
+  <si>
+    <t>los factores que influyen en el rendimiento de los modelos basados en datos y de los algoritmos inteligentes de las soluciones tecnológicas</t>
+  </si>
+  <si>
+    <t>los parámetros de modelos basados en datos y de los algoritmos inteligentes en las soluciones tecnológicas</t>
+  </si>
+  <si>
+    <t>los principios y metodologías de diseño de los modelos y de las arquitecturas de datos de las soluciones tecnológicas</t>
+  </si>
+  <si>
+    <t>prototipos de soluciones tecnológicas que integran datos y algoritmos inteligentes</t>
+  </si>
+  <si>
+    <t>UC1</t>
+  </si>
+  <si>
+    <t>UC3</t>
+  </si>
+  <si>
+    <t>los principios técnicos y tecnológiocos sistemas inteligentes basados en datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> la necesidad de la consideración de los aspectos éticos y legales en la adaptación de sistemas tecnológicos</t>
+  </si>
+  <si>
+    <t>el rendimiento de los principios técnicos y tecnológicos de los sistemas implementados</t>
+  </si>
+  <si>
+    <t>principios técnicos y tecnológicos de los  sistemas basados en datos y algoritmos inteligentes</t>
+  </si>
+  <si>
+    <t>los principios de arquitectura y diseño de software de sistemas basados en datos y algoritmos inteligentes</t>
+  </si>
+  <si>
+    <t>componentes de software para la integración de modelos basados en datos y de algoritmos inteligentes</t>
+  </si>
+  <si>
+    <t>la importancia de la visión sistémica en el desarrollo de soluciones tecnológicas basadas en datos y algoritmos inteligentes</t>
+  </si>
+  <si>
+    <t>los marcos de trabajo y las metodologías aplicadas en los informes de evaluación de proyectos tecnológicos</t>
+  </si>
+  <si>
+    <t>reportes ejecutivos que integren el análisis de datos y las simulaciones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -648,8 +725,23 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -662,8 +754,32 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -815,72 +931,168 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1096,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -1117,15 +1329,15 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1142,7 +1354,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A3" s="20"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1156,38 +1368,38 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="25" customFormat="1" ht="81.599999999999994" customHeight="1">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:10" s="17" customFormat="1" ht="81.599999999999994" customHeight="1">
+      <c r="A4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="24" t="s">
+      <c r="D4" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="21" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="28"/>
     </row>
     <row r="6" spans="1:10" ht="29.25" customHeight="1">
       <c r="A6" s="7" t="s">
@@ -1221,53 +1433,53 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="25" customFormat="1" ht="78.599999999999994" customHeight="1">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:10" s="17" customFormat="1" ht="78.599999999999994" customHeight="1">
+      <c r="A7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="H7" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="J7" s="24" t="s">
+      <c r="I7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="16" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="21" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="23"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="28"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1">
       <c r="A9" s="12" t="s">
@@ -1302,10 +1514,10 @@
         <v>30</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>57</v>
+        <v>62</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>134</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>33</v>
@@ -1315,10 +1527,10 @@
         <v>34</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>66</v>
+        <v>56</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>136</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>33</v>
@@ -1330,10 +1542,10 @@
         <v>36</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>39</v>
@@ -1343,10 +1555,10 @@
         <v>40</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>68</v>
+        <v>37</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>39</v>
@@ -1358,10 +1570,10 @@
         <v>43</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>59</v>
+        <v>65</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>135</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>46</v>
@@ -1371,10 +1583,10 @@
         <v>47</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>70</v>
+        <v>57</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>137</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>46</v>
@@ -2388,7 +2600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34312070-4BCF-4CDB-B449-C479DB9BF40E}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -2409,15 +2621,15 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2434,7 +2646,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A3" s="20"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
@@ -2448,38 +2660,38 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="25" customFormat="1" ht="66" customHeight="1" thickBot="1">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:10" s="17" customFormat="1" ht="66" customHeight="1" thickBot="1">
+      <c r="A4" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>74</v>
+      <c r="B4" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="21" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="28"/>
     </row>
     <row r="6" spans="1:10" ht="29.25" customHeight="1">
       <c r="A6" s="7" t="s">
@@ -2513,53 +2725,53 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="25" customFormat="1" ht="58.8" customHeight="1" thickBot="1">
-      <c r="A7" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" s="24" t="s">
+    <row r="7" spans="1:10" s="17" customFormat="1" ht="58.8" customHeight="1" thickBot="1">
+      <c r="A7" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="J7" s="24" t="s">
-        <v>74</v>
+      <c r="C7" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="21" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="23"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="28"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1">
       <c r="A9" s="12" t="s">
@@ -2591,26 +2803,26 @@
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1">
       <c r="A10" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>98</v>
+        <v>72</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>140</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="26" t="s">
-        <v>105</v>
+        <v>75</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>144</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>33</v>
@@ -2619,26 +2831,26 @@
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1">
       <c r="A11" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>99</v>
+        <v>73</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>141</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="26" t="s">
-        <v>106</v>
+        <v>76</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>146</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>39</v>
@@ -2647,26 +2859,26 @@
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1">
       <c r="A12" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>100</v>
+        <v>74</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>46</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="G12" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="H12" s="26" t="s">
-        <v>107</v>
+        <v>77</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>46</v>
@@ -3670,7 +3882,7 @@
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="F8:J8"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <legacyDrawing r:id="rId1"/>
@@ -3681,7 +3893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A850B921-60A3-4DFE-8A55-217D50109094}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -3702,15 +3914,15 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -3727,7 +3939,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A3" s="20"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
@@ -3741,38 +3953,38 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="25" customFormat="1" ht="66" customHeight="1" thickBot="1">
-      <c r="A4" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>110</v>
+    <row r="4" spans="1:10" s="17" customFormat="1" ht="66" customHeight="1" thickBot="1">
+      <c r="A4" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="21" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="28"/>
     </row>
     <row r="6" spans="1:10" ht="29.25" customHeight="1">
       <c r="A6" s="7" t="s">
@@ -3806,53 +4018,53 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="25" customFormat="1" ht="58.8" customHeight="1" thickBot="1">
-      <c r="A7" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="J7" s="27" t="s">
-        <v>110</v>
+    <row r="7" spans="1:10" s="17" customFormat="1" ht="58.8" customHeight="1" thickBot="1">
+      <c r="A7" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="21" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="23"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="28"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1">
       <c r="A9" s="12" t="s">
@@ -3884,26 +4096,26 @@
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1">
       <c r="A10" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>115</v>
+        <v>81</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="G10" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="H10" s="26" t="s">
-        <v>122</v>
+        <v>84</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>147</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>33</v>
@@ -3912,26 +4124,26 @@
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1">
       <c r="A11" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>116</v>
+        <v>82</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>103</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="26" t="s">
-        <v>123</v>
+        <v>85</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>109</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>39</v>
@@ -3940,26 +4152,26 @@
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1">
       <c r="A12" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>118</v>
+        <v>83</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>105</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>46</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="G12" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="H12" s="26" t="s">
-        <v>125</v>
+        <v>86</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>148</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>46</v>
@@ -4963,7 +5175,7 @@
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="F8:J8"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <legacyDrawing r:id="rId1"/>
@@ -4971,6 +5183,190 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{026A1BB4-B1EF-44B3-B2E2-D5FE0DA4E90C}">
+  <sheetPr codeName="Hoja1"/>
+  <dimension ref="B2:M10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="5" max="5" width="2.109375" style="31" customWidth="1"/>
+    <col min="9" max="9" width="1.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13">
+      <c r="B2" s="29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13">
+      <c r="B3" s="29"/>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="B4" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+    </row>
+    <row r="5" spans="2:13" ht="3.6" customHeight="1">
+      <c r="J5" s="30"/>
+    </row>
+    <row r="6" spans="2:13" s="17" customFormat="1" ht="56.4" customHeight="1">
+      <c r="B6" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="J6" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="K6" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="L6" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="M6" s="42" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" s="17" customFormat="1" ht="56.4" customHeight="1">
+      <c r="B7" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="J7" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="K7" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="M7" s="42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" s="32" customFormat="1" ht="56.4" customHeight="1">
+      <c r="B8" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="F8" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="J8" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="36"/>
+    </row>
+    <row r="9" spans="2:13" s="17" customFormat="1" ht="56.4" customHeight="1">
+      <c r="B9" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="J9" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="K9" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="L9" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="M9" s="44" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" s="17" customFormat="1" ht="56.4" customHeight="1">
+      <c r="B10" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="J10" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" location="page=9.33" xr:uid="{A64DAD6E-AD20-4DBE-AB37-0C95A658E4B8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J990"/>
   <sheetViews>
@@ -4995,15 +5391,15 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -5020,7 +5416,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A3" s="20"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
@@ -5052,20 +5448,20 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="21" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="28"/>
     </row>
     <row r="6" spans="1:10" ht="29.25" customHeight="1">
       <c r="A6" s="7" t="s">
@@ -5132,20 +5528,20 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="21" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="23"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="28"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1">
       <c r="A9" s="12" t="s">

</xml_diff>